<commit_message>
add comments on components
</commit_message>
<xml_diff>
--- a/Eagle files/BOM_Project_design_v1.0.xlsx
+++ b/Eagle files/BOM_Project_design_v1.0.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinsin/Documents/plant4you/Eagle files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\product_design\plant4you\Eagle files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Project_design_v1.0" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>Qty</t>
   </si>
@@ -246,12 +246,54 @@
   </si>
   <si>
     <t>CN1</t>
+  </si>
+  <si>
+    <t>passif components</t>
+  </si>
+  <si>
+    <t>connector</t>
+  </si>
+  <si>
+    <t>temperature sensor</t>
+  </si>
+  <si>
+    <t>battery regulation</t>
+  </si>
+  <si>
+    <t>brightness sensor</t>
+  </si>
+  <si>
+    <t>transistor NMOS</t>
+  </si>
+  <si>
+    <t>RGB LED</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>soil moisture sensor</t>
+  </si>
+  <si>
+    <t>micro precessor</t>
+  </si>
+  <si>
+    <t>ampli op</t>
+  </si>
+  <si>
+    <t>NMOS transistor</t>
+  </si>
+  <si>
+    <t>Micro-USB B Receptacle</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -281,8 +323,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,6 +340,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -559,22 +610,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,8 +642,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4</v>
       </c>
@@ -607,8 +662,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -624,8 +682,9 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -641,8 +700,9 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -658,8 +718,9 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -675,8 +736,9 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -692,8 +754,9 @@
       <c r="E7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -709,8 +772,9 @@
       <c r="E8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>9</v>
       </c>
@@ -726,8 +790,9 @@
       <c r="E9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
@@ -743,8 +808,9 @@
       <c r="E10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -760,8 +826,11 @@
       <c r="E11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -777,8 +846,11 @@
       <c r="E12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -794,8 +866,11 @@
       <c r="E13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -811,8 +886,11 @@
       <c r="E14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>4</v>
       </c>
@@ -828,8 +906,11 @@
       <c r="E15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -845,8 +926,11 @@
       <c r="E16" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -862,8 +946,11 @@
       <c r="E17" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>8</v>
       </c>
@@ -879,8 +966,11 @@
       <c r="E18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
@@ -896,8 +986,11 @@
       <c r="E19" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -913,8 +1006,11 @@
       <c r="E20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -930,8 +1026,11 @@
       <c r="E21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -947,8 +1046,15 @@
       <c r="E22" t="s">
         <v>72</v>
       </c>
+      <c r="F22" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F2:F10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
schematics design uptaded and adjusted for exportation for the MS2
</commit_message>
<xml_diff>
--- a/Eagle files/BOM_Project_design_v1.0.xlsx
+++ b/Eagle files/BOM_Project_design_v1.0.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_Project_design_v1.0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -453,6 +453,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -478,9 +481,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -526,16 +526,16 @@
     <filterColumn colId="7" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="8">
-    <tableColumn id="1" name="Qty" dataDxfId="15" totalsRowDxfId="7"/>
-    <tableColumn id="2" name="Value" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="3" name="Part Num" dataDxfId="13" totalsRowDxfId="5"/>
-    <tableColumn id="4" name="Package" dataDxfId="12" totalsRowDxfId="4"/>
-    <tableColumn id="5" name="Parts" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="8" name="Price / u [CHF]" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="7" name="Price [CHF]" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="1">
+    <tableColumn id="1" name="Qty" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="2" name="Value" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" name="Part Num" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="4" name="Package" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="5" name="Parts" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="8" name="Price / u [CHF]" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" name="Price [CHF]" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="2">
       <totalsRowFormula>SUM(Tableau1[Price '[CHF']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Comments" dataDxfId="10" totalsRowDxfId="0"/>
+    <tableColumn id="6" name="Comments" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -807,7 +807,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>